<commit_message>
Se agregó el diagrama de robustez del CU15 - Registrar venta y se corrigió su descripción de CU, además de corrección al reporte de errores
</commit_message>
<xml_diff>
--- a/ReporteDeErrores.xlsx
+++ b/ReporteDeErrores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\OneDrive\Escritorio\Proyectos\DesarrolloSoftware\SAMS_Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escuela\7° Semestre\Desarrollo de Software\Proyecto\SAMS_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A9B5AE-F066-4140-8F52-E04B0A9E731C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531BB0E4-5D6C-415E-9F7A-9D1DF5522D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{90DA4DCB-4B44-4051-ABD0-0E91DF82B625}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
   <si>
     <t>cesar</t>
   </si>
@@ -65,9 +65,6 @@
     <t>cristof</t>
   </si>
   <si>
-    <t>feddback</t>
-  </si>
-  <si>
     <t>Resolucion</t>
   </si>
   <si>
@@ -243,6 +240,12 @@
   </si>
   <si>
     <t>Pendiente</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>descripciones de caso de uso, Diagramas de Robustez, Diagramas de Sequencia</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,7 @@
     <tableColumn id="2" xr3:uid="{1C164519-FA79-4FEB-8B72-6FCBFFE6E84C}" name="problema" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{76EF2905-3BE7-4975-A376-8897FA281E82}" name="nombre"/>
     <tableColumn id="4" xr3:uid="{1207E0CD-B87B-4520-9D2D-344213EE6C71}" name="artefacto afecta" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{4AE01FB9-6F14-4E18-A07C-69DE37EB88F6}" name="feddback"/>
+    <tableColumn id="5" xr3:uid="{4AE01FB9-6F14-4E18-A07C-69DE37EB88F6}" name="feedback"/>
     <tableColumn id="6" xr3:uid="{FCF699A7-8468-4559-8055-989800C7CD9B}" name="Resolucion" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{C90B9980-FCDC-41E8-99BE-E84316B812AC}" name="Estado"/>
   </tableColumns>
@@ -671,8 +674,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="81" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E22:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,7 +691,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -700,13 +703,13 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -720,16 +723,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -737,22 +740,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -760,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -769,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -777,19 +780,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -797,22 +800,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>18</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -820,19 +823,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -840,22 +843,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>18</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -863,19 +866,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -883,22 +886,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>18</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -906,22 +909,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -929,22 +932,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -952,22 +955,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" t="s">
         <v>48</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -975,22 +978,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
         <v>18</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -998,13 +1001,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1012,22 +1015,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>18</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1035,22 +1038,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" t="s">
         <v>18</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1058,42 +1061,42 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1101,22 +1104,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" t="s">
         <v>18</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1129,23 +1132,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="add8837a-384a-4016-82b1-1ac351df06b6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007C29FB0312039C43A3E25ACCB758F0F1" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a831f32d98793a73fa3e65f0c5c19796">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="add8837a-384a-4016-82b1-1ac351df06b6" xmlns:ns4="7f363fac-3372-41f2-8a27-58fa335250c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c3faef4219cda1ba8d7cd8aa18f70377" ns3:_="" ns4:_="">
     <xsd:import namespace="add8837a-384a-4016-82b1-1ac351df06b6"/>
@@ -1384,32 +1370,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EB254F5-E46E-46C7-B524-653816385C80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7f363fac-3372-41f2-8a27-58fa335250c4"/>
-    <ds:schemaRef ds:uri="add8837a-384a-4016-82b1-1ac351df06b6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F056FA1-1F1E-496B-8A50-A373C2863001}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="add8837a-384a-4016-82b1-1ac351df06b6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F8173D9-631B-4BFB-8881-1E8DC4112881}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1426,4 +1404,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F056FA1-1F1E-496B-8A50-A373C2863001}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EB254F5-E46E-46C7-B524-653816385C80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f363fac-3372-41f2-8a27-58fa335250c4"/>
+    <ds:schemaRef ds:uri="add8837a-384a-4016-82b1-1ac351df06b6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix(CU-12 Editar empleado): corregida descripcion de acuerdo con las correcciones del lunes 23 de septiembre
</commit_message>
<xml_diff>
--- a/ReporteDeErrores.xlsx
+++ b/ReporteDeErrores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wizar\Desktop\SAMS_Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raul\Desktop\SAMS_Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC8D48D-ACA0-4258-82A0-7D45B883B22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC41BB19-2958-4FC3-975D-5F32D0D7F38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{90DA4DCB-4B44-4051-ABD0-0E91DF82B625}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{90DA4DCB-4B44-4051-ABD0-0E91DF82B625}"/>
   </bookViews>
   <sheets>
     <sheet name="Primera Entrega" sheetId="1" r:id="rId1"/>
@@ -291,18 +291,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF6D70"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -316,7 +309,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFF5B5B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -324,76 +317,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5B5B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3F44"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -440,12 +363,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{916A10CC-03F2-40F4-9511-F1945F2FD4B6}" name="Tabla1" displayName="Tabla1" ref="A1:G20" totalsRowShown="0">
   <autoFilter ref="A1:G20" xr:uid="{916A10CC-03F2-40F4-9511-F1945F2FD4B6}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BEA0304E-98EA-484C-9C70-8AD83D19BDA2}" name="No." dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{1C164519-FA79-4FEB-8B72-6FCBFFE6E84C}" name="Problema" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{76EF2905-3BE7-4975-A376-8897FA281E82}" name="Detectado" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{1207E0CD-B87B-4520-9D2D-344213EE6C71}" name="Artefacto(s)" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{4AE01FB9-6F14-4E18-A07C-69DE37EB88F6}" name="Resuelto" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{FCF699A7-8468-4559-8055-989800C7CD9B}" name="Resolucion" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{BEA0304E-98EA-484C-9C70-8AD83D19BDA2}" name="No." dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{1C164519-FA79-4FEB-8B72-6FCBFFE6E84C}" name="Problema" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{76EF2905-3BE7-4975-A376-8897FA281E82}" name="Detectado" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{1207E0CD-B87B-4520-9D2D-344213EE6C71}" name="Artefacto(s)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{4AE01FB9-6F14-4E18-A07C-69DE37EB88F6}" name="Resuelto" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{FCF699A7-8468-4559-8055-989800C7CD9B}" name="Resolucion" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{C90B9980-FCDC-41E8-99BE-E84316B812AC}" name="Estado"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -774,22 +697,22 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="81" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -812,7 +735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -835,7 +758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -858,7 +781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -875,7 +798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -893,7 +816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -916,7 +839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -936,7 +859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -959,7 +882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -976,7 +899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -999,7 +922,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1022,7 +945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1045,7 +968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1068,7 +991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1091,7 +1014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1105,7 +1028,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1128,7 +1051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1148,10 +1071,10 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1171,7 +1094,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1194,7 +1117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1217,25 +1140,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
-      <formula>"Resuelto"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Pendiente"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Aceptado">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Rechazado"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Aceptado">
       <formula>NOT(ISERROR(SEARCH("Aceptado",G1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
-      <formula>"Rechazado"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
-      <formula>"Pendiente"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Resuelto"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1247,23 +1170,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="add8837a-384a-4016-82b1-1ac351df06b6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007C29FB0312039C43A3E25ACCB758F0F1" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a831f32d98793a73fa3e65f0c5c19796">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="add8837a-384a-4016-82b1-1ac351df06b6" xmlns:ns4="7f363fac-3372-41f2-8a27-58fa335250c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c3faef4219cda1ba8d7cd8aa18f70377" ns3:_="" ns4:_="">
     <xsd:import namespace="add8837a-384a-4016-82b1-1ac351df06b6"/>
@@ -1502,32 +1408,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EB254F5-E46E-46C7-B524-653816385C80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7f363fac-3372-41f2-8a27-58fa335250c4"/>
-    <ds:schemaRef ds:uri="add8837a-384a-4016-82b1-1ac351df06b6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F056FA1-1F1E-496B-8A50-A373C2863001}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="add8837a-384a-4016-82b1-1ac351df06b6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F8173D9-631B-4BFB-8881-1E8DC4112881}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1544,4 +1442,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F056FA1-1F1E-496B-8A50-A373C2863001}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EB254F5-E46E-46C7-B524-653816385C80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f363fac-3372-41f2-8a27-58fa335250c4"/>
+    <ds:schemaRef ds:uri="add8837a-384a-4016-82b1-1ac351df06b6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>